<commit_message>
Actualizo productos, nombres e imágenes en materiales
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facun\OneDrive\Escritorio\fuegodeatenea_web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facun\OneDrive\Escritorio\Miprimerapaginafsosa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="9048"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="HOJA-FINAL" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="169">
   <si>
     <t>nombre</t>
   </si>
@@ -503,6 +503,33 @@
   </si>
   <si>
     <t>CONCATENACION</t>
+  </si>
+  <si>
+    <t>descarga (1)</t>
+  </si>
+  <si>
+    <t>Sahumerio Mixto</t>
+  </si>
+  <si>
+    <t>GENÉRICO</t>
+  </si>
+  <si>
+    <t>Pack de sahumerios mixtos. Imagen muestra packaging simple, color variado.</t>
+  </si>
+  <si>
+    <t>descarga (1).jpg</t>
+  </si>
+  <si>
+    <t>descarga (2)</t>
+  </si>
+  <si>
+    <t>Sahumerio Clásico</t>
+  </si>
+  <si>
+    <t>Sahumerio clásico en caja. Etiqueta visible, aromas varios.</t>
+  </si>
+  <si>
+    <t>descarga (2).jpg</t>
   </si>
 </sst>
 </file>
@@ -579,7 +606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -587,7 +614,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -597,7 +623,6 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -909,33 +934,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="34.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="28.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="26.77734375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.6640625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="5.6640625" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="4" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>60</v>
       </c>
@@ -951,7 +977,7 @@
       <c r="E1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>64</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -985,882 +1011,950 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="6">
         <v>2800</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4">
-        <v>1</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3">
+        <v>1</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>2800</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4">
-        <v>1</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>2800</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4">
-        <v>1</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <v>2800</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4">
-        <v>1</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3">
+        <v>1</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>2800</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4" t="s">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4">
-        <v>1</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3">
+        <v>1</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>2800</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4">
-        <v>1</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="N7" s="3"/>
+      <c r="O7" s="3">
+        <v>1</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <v>2800</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="O8" s="4">
-        <v>1</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="O8" s="3">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <v>2800</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4">
-        <v>1</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <v>2800</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5" t="s">
+      <c r="H10" s="3"/>
+      <c r="I10" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4">
-        <v>1</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <v>2800</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5" t="s">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3">
+        <v>1</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>2800</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4" t="s">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4">
-        <v>1</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <v>2800</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4">
-        <v>1</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3">
+        <v>1</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <v>2800</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4" t="s">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4">
-        <v>1</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="N14" s="3"/>
+      <c r="O14" s="3">
+        <v>1</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="6">
         <v>2800</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4">
-        <v>1</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3">
+        <v>1</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="6">
         <v>2800</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4" t="s">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4">
-        <v>1</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3">
+        <v>1</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>2200</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4">
-        <v>1</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3">
+        <v>1</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>2200</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4">
-        <v>1</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3">
+        <v>1</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>2200</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4" t="s">
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4">
-        <v>1</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3">
+        <v>1</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>2000</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4">
-        <v>1</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3">
+        <v>1</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>2000</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4" t="s">
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4">
-        <v>1</v>
-      </c>
-      <c r="P21" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3">
+        <v>1</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>4000</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4">
-        <v>1</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3">
+        <v>1</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>4000</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4" t="s">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4">
-        <v>1</v>
-      </c>
-      <c r="P23" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3">
+        <v>1</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <v>4000</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4" t="s">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4">
-        <v>1</v>
-      </c>
-      <c r="P24" s="4" t="s">
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3">
+        <v>1</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>30</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="7">
+        <v>4200</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="O25" s="3">
+        <v>1</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>31</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" s="7">
+        <v>4200</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="O26" s="3">
+        <v>1</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1868,21 +1962,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:C27"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1996,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1919,7 +2013,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1927,7 +2021,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1935,7 +2029,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1946,7 +2040,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1957,7 +2051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1968,7 +2062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1979,7 +2073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1990,7 +2084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2001,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2012,7 +2106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2023,7 +2117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -2034,7 +2128,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -2045,7 +2139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2056,7 +2150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2067,7 +2161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -2078,7 +2172,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -2089,7 +2183,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -2100,7 +2194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2111,7 +2205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2122,7 +2216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2133,7 +2227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -2144,7 +2238,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2155,7 +2249,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2166,7 +2260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2177,7 +2271,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2188,7 +2282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2199,7 +2293,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2210,7 +2304,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2221,7 +2315,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2232,7 +2326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -2243,7 +2337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
WIP: Avances en catálogo, seguimos mañana
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="177">
   <si>
     <t>nombre</t>
   </si>
@@ -247,9 +247,6 @@
     <t>ALAUKIK</t>
   </si>
   <si>
-    <t xml:space="preserve">Colección importada de la india, contenido 50 varillas .Duracion 1:30/2 horas </t>
-  </si>
-  <si>
     <t>Limpia Casa</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>Imagen 6</t>
   </si>
   <si>
-    <t>Sahumerio Crystal Esent Aroma - LABRADORITA</t>
-  </si>
-  <si>
     <t>Negro y Oro</t>
   </si>
   <si>
@@ -316,9 +310,6 @@
     <t>White Widow</t>
   </si>
   <si>
-    <t>Cannabis THC</t>
-  </si>
-  <si>
     <t>Tropicana Cookies</t>
   </si>
   <si>
@@ -334,9 +325,6 @@
     <t>AROMANZA</t>
   </si>
   <si>
-    <t>Palo Santo Buena Onda</t>
-  </si>
-  <si>
     <t>Energia Limpia</t>
   </si>
   <si>
@@ -355,15 +343,9 @@
     <t>Champa</t>
   </si>
   <si>
-    <t>Colección importada de la india, contenido 50 varillas .Duracion 1 hora</t>
-  </si>
-  <si>
     <t>30min</t>
   </si>
   <si>
-    <t xml:space="preserve">Sahumerio Hecho a mano </t>
-  </si>
-  <si>
     <t>ALAUKIK_Limpia_Casa.jpg</t>
   </si>
   <si>
@@ -514,9 +496,6 @@
     <t>GENÉRICO</t>
   </si>
   <si>
-    <t>Pack de sahumerios mixtos. Imagen muestra packaging simple, color variado.</t>
-  </si>
-  <si>
     <t>descarga (1).jpg</t>
   </si>
   <si>
@@ -526,10 +505,55 @@
     <t>Sahumerio Clásico</t>
   </si>
   <si>
-    <t>Sahumerio clásico en caja. Etiqueta visible, aromas varios.</t>
-  </si>
-  <si>
     <t>descarga (2).jpg</t>
+  </si>
+  <si>
+    <t>Sahumerio especial para limpieza energética de ambientes. Ideal para renovar el aire y atraer bienestar. Pack de 50 varillas, duración 2 horas.</t>
+  </si>
+  <si>
+    <t>Aroma lavanda importado. Perfecto para relajarse, crear ambientes calmados y acompañar rutinas de descanso. Varillas largas (50u) que perfuman el espacio por hasta 2 horas.</t>
+  </si>
+  <si>
+    <t>Sahumerio de canela, clásico para atraer energía positiva y purificar el aire. Ideal para tu hogar u oficina. Pack de 50 varillas, duración extendida.</t>
+  </si>
+  <si>
+    <t>Sahumerio de jazmín, aroma dulce y floral. Usalo para potenciar buenas vibras y decorar tu ambiente. 50 varillas, perfume intenso por más de 1 hora.</t>
+  </si>
+  <si>
+    <t>Varillas de sahumerio importadas con aroma melón. Perfume fresco y frutal pensado para ambientar y dar energía a tu espacio. 50 varillas, larga duración.</t>
+  </si>
+  <si>
+    <t>Sahumerio aroma cannabis especial. Perfume moderno y diferente, duración 1 hora.</t>
+  </si>
+  <si>
+    <t>Sahumerio cannabis Tropicana Cookies. Aroma único, ideal para ambientar reuniones o momentos creativos. 1 hora de efecto.</t>
+  </si>
+  <si>
+    <t>Pack de sahumerios surtidos. Ideal para probar diferentes fragancias y renovar la energía de tu ambiente.</t>
+  </si>
+  <si>
+    <t>Pack clásico de sahumerios, aromas varios. Perfume tu espacio con tradición y variedad. Duración estándar, 1 hora.</t>
+  </si>
+  <si>
+    <t>Sahumerios premium con piedra semipreciosa verdadera. Cada uno ayuda a potenciar la energía y armonía del ambiente, combinando la aromaterapia con el poder natural de los cristales. El detalle ideal para regalar bienestar. Pack de varillas, fragancia especial de larga duración.</t>
+  </si>
+  <si>
+    <t>Sahumerios importados de la India, reconocidos por su excelente calidad y aromas auténticos. Varillas largas, fragancia persistente, ideales para quienes buscan un aire exótico y relajante todos los días.</t>
+  </si>
+  <si>
+    <t>Sahumerio artesano diseñado para activar la intuición y potenciar la claridad mental. Ideal para prácticas de yoga, meditación y búsqueda interior. Fragancia envolvente que ayuda a conectar con tu sabiduría interna.</t>
+  </si>
+  <si>
+    <t>Sahumerio especial para rituales con cacao. Crea un ambiente cálido y espiritual para ceremonias, meditaciones y momentos de conexión profunda. Aroma ancestral que invita a abrir el corazón y disfrutar instantes de bienestar.</t>
+  </si>
+  <si>
+    <t>Aroma equilibrado pensado para acompañar rutinas de yoga, relajación y mindfulness. Ayuda a focalizar la energía y a crear un espacio armónico para la práctica personal. Varillas gruesas, duración prolongada.</t>
+  </si>
+  <si>
+    <t>Sahumerios con fragancia a frutos rojos, ideal para perfumar tu casa con un aroma dulce y moderno. Crea un ambiente alegre, fresco y con el toque especial de la naturaleza. Varillas de larga duración para acompañar cada día.</t>
+  </si>
+  <si>
+    <t>Sahumerio formulado para limpiar y renovar la energía del hogar. Aroma fresco y revitalizante, recomendado para ambientes cargados, cambios y nuevos comienzos. Usalo para atraer armonía y bienestar donde más lo necesitas.</t>
   </si>
 </sst>
 </file>
@@ -540,7 +564,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,6 +586,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -606,29 +636,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -937,23 +964,22 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="4" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="168.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="29.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.7109375" style="4" customWidth="1"/>
@@ -966,7 +992,7 @@
         <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>61</v>
@@ -977,11 +1003,11 @@
       <c r="E1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>65</v>
@@ -996,13 +1022,13 @@
         <v>68</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>69</v>
@@ -1012,908 +1038,908 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>74</v>
+      <c r="E2" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="F2" s="6">
         <v>2800</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3">
-        <v>1</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="G2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5">
+        <v>1</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>74</v>
+      <c r="E3" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="F3" s="6">
         <v>2800</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5">
+        <v>1</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3">
-        <v>1</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>74</v>
+      <c r="E4" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="F4" s="6">
         <v>2800</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3">
-        <v>1</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="G4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>74</v>
+      <c r="E5" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="F5" s="6">
         <v>2800</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3">
-        <v>1</v>
-      </c>
-      <c r="P5" s="3" t="s">
+      <c r="G5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>74</v>
+      <c r="E6" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="F6" s="6">
         <v>2800</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3">
-        <v>1</v>
-      </c>
-      <c r="P6" s="3" t="s">
+      <c r="G6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5">
+        <v>1</v>
+      </c>
+      <c r="P6" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="B7" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>74</v>
+      <c r="E7" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="F7" s="6">
         <v>2800</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3">
-        <v>1</v>
-      </c>
-      <c r="P7" s="3" t="s">
+      <c r="G7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5">
+        <v>1</v>
+      </c>
+      <c r="P7" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>74</v>
+      <c r="E8" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="F8" s="6">
         <v>2800</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="O8" s="3">
-        <v>1</v>
-      </c>
-      <c r="P8" s="3" t="s">
+      <c r="G8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1</v>
+      </c>
+      <c r="P8" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>86</v>
+      <c r="B9" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="F9" s="6">
         <v>2800</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>89</v>
+      <c r="G9" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3">
-        <v>1</v>
-      </c>
-      <c r="P9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+      <c r="P9" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>86</v>
+      <c r="B10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="F10" s="6">
         <v>2800</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5">
+        <v>1</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3">
-        <v>1</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>86</v>
+      <c r="D11" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="F11" s="6">
         <v>2800</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="G11" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3">
-        <v>1</v>
-      </c>
-      <c r="P11" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5">
+        <v>1</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>86</v>
+      <c r="B12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="F12" s="6">
         <v>2800</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3">
-        <v>1</v>
-      </c>
-      <c r="P12" s="3" t="s">
+      <c r="G12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5">
+        <v>1</v>
+      </c>
+      <c r="P12" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>86</v>
+      <c r="B13" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="F13" s="6">
         <v>2800</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3">
-        <v>1</v>
-      </c>
-      <c r="P13" s="3" t="s">
+      <c r="G13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5">
+        <v>1</v>
+      </c>
+      <c r="P13" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>86</v>
+      <c r="B14" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="F14" s="6">
         <v>2800</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3">
-        <v>1</v>
-      </c>
-      <c r="P14" s="3" t="s">
+      <c r="G14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5">
+        <v>1</v>
+      </c>
+      <c r="P14" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>95</v>
+      <c r="B15" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>97</v>
+        <v>166</v>
       </c>
       <c r="F15" s="6">
         <v>2800</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3">
-        <v>1</v>
-      </c>
-      <c r="P15" s="3" t="s">
+      <c r="G15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5">
+        <v>1</v>
+      </c>
+      <c r="P15" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B16" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="D16" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="E16" s="4" t="s">
-        <v>97</v>
+        <v>167</v>
       </c>
       <c r="F16" s="6">
         <v>2800</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3">
-        <v>1</v>
-      </c>
-      <c r="P16" s="3" t="s">
+      <c r="G16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5">
+        <v>1</v>
+      </c>
+      <c r="P16" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>95</v>
+      <c r="B17" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>112</v>
+        <v>173</v>
       </c>
       <c r="F17" s="7">
         <v>2200</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3">
-        <v>1</v>
-      </c>
-      <c r="P17" s="3" t="s">
+      <c r="G17" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5">
+        <v>1</v>
+      </c>
+      <c r="P17" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>95</v>
+      <c r="B18" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>112</v>
+        <v>172</v>
       </c>
       <c r="F18" s="7">
         <v>2200</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3">
-        <v>1</v>
-      </c>
-      <c r="P18" s="3" t="s">
+      <c r="G18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5">
+        <v>1</v>
+      </c>
+      <c r="P18" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>95</v>
+      <c r="B19" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="F19" s="7">
         <v>2200</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3">
-        <v>1</v>
-      </c>
-      <c r="P19" s="3" t="s">
+      <c r="G19" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5">
+        <v>1</v>
+      </c>
+      <c r="P19" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>102</v>
+      <c r="B20" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
       <c r="F20" s="7">
         <v>2000</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3">
-        <v>1</v>
-      </c>
-      <c r="P20" s="3" t="s">
+      <c r="G20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5">
+        <v>1</v>
+      </c>
+      <c r="P20" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>102</v>
+      <c r="B21" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>103</v>
+        <v>176</v>
       </c>
       <c r="F21" s="7">
         <v>2000</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3">
-        <v>1</v>
-      </c>
-      <c r="P21" s="3" t="s">
+      <c r="G21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5">
+        <v>1</v>
+      </c>
+      <c r="P21" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>110</v>
+      <c r="B22" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="F22" s="7">
         <v>4000</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3">
-        <v>1</v>
-      </c>
-      <c r="P22" s="3" t="s">
+      <c r="G22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5">
+        <v>1</v>
+      </c>
+      <c r="P22" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>110</v>
+      <c r="B23" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="F23" s="7">
         <v>4000</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3">
-        <v>1</v>
-      </c>
-      <c r="P23" s="3" t="s">
+      <c r="G23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5">
+        <v>1</v>
+      </c>
+      <c r="P23" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>110</v>
+      <c r="B24" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="F24" s="7">
         <v>4000</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3">
-        <v>1</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="G24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5">
+        <v>1</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
         <v>30</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="F25" s="7">
         <v>4200</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="O25" s="3">
-        <v>1</v>
-      </c>
-      <c r="P25" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O25" s="5">
+        <v>1</v>
+      </c>
+      <c r="P25" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1922,33 +1948,33 @@
         <v>31</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F26" s="7">
         <v>4200</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="O26" s="3">
-        <v>1</v>
-      </c>
-      <c r="P26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="O26" s="5">
+        <v>1</v>
+      </c>
+      <c r="P26" s="5" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>

<commit_message>
traducir checkout al español
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -490,21 +490,12 @@
     <t>descarga (1)</t>
   </si>
   <si>
-    <t>Sahumerio Mixto</t>
-  </si>
-  <si>
-    <t>GENÉRICO</t>
-  </si>
-  <si>
     <t>descarga (1).jpg</t>
   </si>
   <si>
     <t>descarga (2)</t>
   </si>
   <si>
-    <t>Sahumerio Clásico</t>
-  </si>
-  <si>
     <t>descarga (2).jpg</t>
   </si>
   <si>
@@ -529,12 +520,6 @@
     <t>Sahumerio cannabis Tropicana Cookies. Aroma único, ideal para ambientar reuniones o momentos creativos. 1 hora de efecto.</t>
   </si>
   <si>
-    <t>Pack de sahumerios surtidos. Ideal para probar diferentes fragancias y renovar la energía de tu ambiente.</t>
-  </si>
-  <si>
-    <t>Pack clásico de sahumerios, aromas varios. Perfume tu espacio con tradición y variedad. Duración estándar, 1 hora.</t>
-  </si>
-  <si>
     <t>Sahumerios premium con piedra semipreciosa verdadera. Cada uno ayuda a potenciar la energía y armonía del ambiente, combinando la aromaterapia con el poder natural de los cristales. El detalle ideal para regalar bienestar. Pack de varillas, fragancia especial de larga duración.</t>
   </si>
   <si>
@@ -554,6 +539,21 @@
   </si>
   <si>
     <t>Sahumerio formulado para limpiar y renovar la energía del hogar. Aroma fresco y revitalizante, recomendado para ambientes cargados, cambios y nuevos comienzos. Usalo para atraer armonía y bienestar donde más lo necesitas.</t>
+  </si>
+  <si>
+    <t>Limpia Hogar</t>
+  </si>
+  <si>
+    <t>Aroma Fusion</t>
+  </si>
+  <si>
+    <t>Meditation </t>
+  </si>
+  <si>
+    <t>Sahumerio formulado para limpiar y renovar la energía del hogar. Aroma fresco, ideal para crear ambientes más puros y armoniosos. Usalo para atraer protección y bienestar a tus espacios. Varillas largas, con fragancia</t>
+  </si>
+  <si>
+    <t>Sahumerio diseñado para la meditación y la espiritualidad. Aroma suave y relajante, perfecto para momentos de paz interior y contemplación. Favorece la armonización del ambiente y el bienestar espiritual. Varillas largas, con fragancia persistente</t>
   </si>
 </sst>
 </file>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,7 @@
         <v>73</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F2" s="6">
         <v>2800</v>
@@ -1089,7 +1089,7 @@
         <v>73</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F3" s="6">
         <v>2800</v>
@@ -1127,7 +1127,7 @@
         <v>73</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F4" s="6">
         <v>2800</v>
@@ -1165,7 +1165,7 @@
         <v>73</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F5" s="6">
         <v>2800</v>
@@ -1203,7 +1203,7 @@
         <v>73</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F6" s="6">
         <v>2800</v>
@@ -1241,7 +1241,7 @@
         <v>73</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F7" s="6">
         <v>2800</v>
@@ -1279,7 +1279,7 @@
         <v>73</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F8" s="6">
         <v>2800</v>
@@ -1317,7 +1317,7 @@
         <v>84</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F9" s="6">
         <v>2800</v>
@@ -1355,7 +1355,7 @@
         <v>84</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F10" s="6">
         <v>2800</v>
@@ -1393,7 +1393,7 @@
         <v>84</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F11" s="6">
         <v>2800</v>
@@ -1431,7 +1431,7 @@
         <v>84</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F12" s="6">
         <v>2800</v>
@@ -1469,7 +1469,7 @@
         <v>84</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F13" s="6">
         <v>2800</v>
@@ -1507,7 +1507,7 @@
         <v>84</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F14" s="6">
         <v>2800</v>
@@ -1545,7 +1545,7 @@
         <v>93</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F15" s="6">
         <v>2800</v>
@@ -1583,7 +1583,7 @@
         <v>93</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F16" s="6">
         <v>2800</v>
@@ -1621,7 +1621,7 @@
         <v>93</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F17" s="7">
         <v>2200</v>
@@ -1659,7 +1659,7 @@
         <v>93</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F18" s="7">
         <v>2200</v>
@@ -1697,7 +1697,7 @@
         <v>93</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F19" s="7">
         <v>2200</v>
@@ -1735,7 +1735,7 @@
         <v>99</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F20" s="7">
         <v>2000</v>
@@ -1773,7 +1773,7 @@
         <v>99</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F21" s="7">
         <v>2000</v>
@@ -1811,7 +1811,7 @@
         <v>102</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F22" s="7">
         <v>4000</v>
@@ -1849,7 +1849,7 @@
         <v>102</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F23" s="7">
         <v>4000</v>
@@ -1887,7 +1887,7 @@
         <v>102</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F24" s="7">
         <v>4000</v>
@@ -1919,13 +1919,13 @@
         <v>154</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="F25" s="7">
         <v>4200</v>
@@ -1934,7 +1934,7 @@
         <v>87</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O25" s="5">
         <v>1</v>
@@ -1948,16 +1948,16 @@
         <v>31</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="F26" s="7">
         <v>4200</v>
@@ -1966,10 +1966,10 @@
         <v>87</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O26" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Actualizo archivo Excel con nueva descripción de sahumerios
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="HOJA-FINAL" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'HOJA-FINAL'!$A$1:$P$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$C$33</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="208">
   <si>
     <t>nombre</t>
   </si>
@@ -238,9 +239,6 @@
     <t>Activo</t>
   </si>
   <si>
-    <t>Sí</t>
-  </si>
-  <si>
     <t>Holadensa Rosa</t>
   </si>
   <si>
@@ -313,12 +311,6 @@
     <t>Tropicana Cookies</t>
   </si>
   <si>
-    <t>Ritual Tercer Ojo</t>
-  </si>
-  <si>
-    <t>Ritual Yoga</t>
-  </si>
-  <si>
     <t>Futos Rojos</t>
   </si>
   <si>
@@ -541,19 +533,121 @@
     <t>Sahumerio formulado para limpiar y renovar la energía del hogar. Aroma fresco y revitalizante, recomendado para ambientes cargados, cambios y nuevos comienzos. Usalo para atraer armonía y bienestar donde más lo necesitas.</t>
   </si>
   <si>
-    <t>Limpia Hogar</t>
-  </si>
-  <si>
-    <t>Aroma Fusion</t>
-  </si>
-  <si>
-    <t>Meditation </t>
-  </si>
-  <si>
     <t>Sahumerio formulado para limpiar y renovar la energía del hogar. Aroma fresco, ideal para crear ambientes más puros y armoniosos. Usalo para atraer protección y bienestar a tus espacios. Varillas largas, con fragancia</t>
   </si>
   <si>
     <t>Sahumerio diseñado para la meditación y la espiritualidad. Aroma suave y relajante, perfecto para momentos de paz interior y contemplación. Favorece la armonización del ambiente y el bienestar espiritual. Varillas largas, con fragancia persistente</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>AROMA FUSION</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Fresa</t>
+  </si>
+  <si>
+    <t>Vainilla</t>
+  </si>
+  <si>
+    <t>Anana</t>
+  </si>
+  <si>
+    <t>Ritual Abundancia</t>
+  </si>
+  <si>
+    <t>Sagrado Tercer Ojo</t>
+  </si>
+  <si>
+    <t>Sagrado Yoga</t>
+  </si>
+  <si>
+    <t>Watermelon</t>
+  </si>
+  <si>
+    <t>Purple Hindu Kush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naranja Pimienta </t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Variedad Aromatica</t>
+  </si>
+  <si>
+    <t>Meditation XL</t>
+  </si>
+  <si>
+    <t>Limpia Hogar XL</t>
+  </si>
+  <si>
+    <t>Black Ice XL</t>
+  </si>
+  <si>
+    <t>Strawberry XL</t>
+  </si>
+  <si>
+    <t>Cool water</t>
+  </si>
+  <si>
+    <t>Manzana Canela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lavanda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strawberry </t>
+  </si>
+  <si>
+    <t>Palo Santo</t>
+  </si>
+  <si>
+    <t>Rosa Vainilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Ice </t>
+  </si>
+  <si>
+    <t>Anana Sobre</t>
+  </si>
+  <si>
+    <t>Rosa Sobre</t>
+  </si>
+  <si>
+    <t>Fantasia Sobre</t>
+  </si>
+  <si>
+    <t>Ojo de Tigre</t>
+  </si>
+  <si>
+    <t>Venturina</t>
+  </si>
+  <si>
+    <t>Sahumerios Surtidos</t>
+  </si>
+  <si>
+    <t>Aqua Fresh</t>
+  </si>
+  <si>
+    <t>VARIAS</t>
+  </si>
+  <si>
+    <t>Sahumerio especial para rituales. Crea un ambiente cálido y espiritual para ceremonias, meditaciones y momentos de conexión profunda. Aroma ancestral que invita a abrir el corazón y disfrutar instantes de bienestar.</t>
+  </si>
+  <si>
+    <t>Sahumerio formulado para limpiar y renovar la energía del hogar. Aroma fresco, ideal para crear ambientes más puros y armoniosos. Usalo para atraer protección y bienestar a tus espacios. Varillas cortas, con fragancia</t>
+  </si>
+  <si>
+    <t>Sahumerio especial para limpieza energética de ambientes. Ideal para renovar el aire y atraer bienestar. Sobre de varillas.</t>
+  </si>
+  <si>
+    <t>Sahumerios hexagonales económicos: fragancias intensas y variadas para perfumar y renovar la energía de cualquier ambiente. Opción práctica y accesible para tu hogar o espacio de trabajo.</t>
   </si>
 </sst>
 </file>
@@ -961,29 +1055,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="168.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="29.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="252.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
@@ -992,7 +1085,7 @@
         <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>61</v>
@@ -1007,7 +1100,7 @@
         <v>64</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>65</v>
@@ -1022,13 +1115,13 @@
         <v>68</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="N1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>69</v>
@@ -1042,25 +1135,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="6">
+        <v>4190</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="H2" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -1069,10 +1162,10 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1080,26 +1173,26 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F3" s="6">
-        <v>2800</v>
+        <v>4190</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -1107,10 +1200,10 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1118,37 +1211,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F4" s="6">
-        <v>2800</v>
+        <v>4190</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1156,37 +1249,37 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F5" s="6">
-        <v>2800</v>
+        <v>4190</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1194,29 +1287,29 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F6" s="6">
-        <v>2800</v>
+        <v>4190</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -1224,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1232,22 +1325,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F7" s="6">
-        <v>2800</v>
+        <v>4190</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -1255,14 +1348,14 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5">
         <v>1</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1270,22 +1363,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F8" s="6">
-        <v>2800</v>
+        <v>4190</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1294,40 +1387,37 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="O8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>137</v>
+      <c r="B9" s="5" t="str">
+        <f>+CONCATENATE(C9," ",D9)</f>
+        <v>Aqua Fresh ALAUKIK</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>85</v>
+        <v>202</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>165</v>
+        <v>72</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F9" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>114</v>
-      </c>
+        <v>4190</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -1335,227 +1425,209 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>138</v>
+      <c r="B10" s="5" t="str">
+        <f t="shared" ref="B10:B16" si="0">+CONCATENATE(C10," ",D10)</f>
+        <v>Mango ALAUKIK</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>165</v>
+        <v>72</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F10" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>4190</v>
+      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="4" t="s">
-        <v>115</v>
-      </c>
+      <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>139</v>
+      <c r="B11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Fresa ALAUKIK</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>165</v>
+        <v>72</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F11" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>4190</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="4" t="s">
-        <v>116</v>
-      </c>
+      <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>140</v>
+      <c r="B12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Vainilla ALAUKIK</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>165</v>
+        <v>72</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F12" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>4190</v>
+      </c>
+      <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>141</v>
+      <c r="B13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Anana ALAUKIK</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>91</v>
+        <v>176</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>165</v>
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="F13" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>4190</v>
+      </c>
+      <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5">
         <v>1</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>142</v>
+      <c r="B14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Anana Sobre ALAUKIK</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>92</v>
+        <v>196</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>165</v>
+        <v>72</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="F14" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>4190</v>
+      </c>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>143</v>
+      <c r="B15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Rosa Sobre ALAUKIK</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>94</v>
+        <v>197</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>163</v>
+        <v>72</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="F15" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>120</v>
-      </c>
+        <v>4190</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -1563,48 +1635,45 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>144</v>
+      <c r="B16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Fantasia Sobre ALAUKIK</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>95</v>
+        <v>198</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>164</v>
+        <v>72</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="F16" s="6">
-        <v>2800</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>4190</v>
+      </c>
+      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="5" t="s">
-        <v>121</v>
-      </c>
+      <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1612,25 +1681,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F17" s="7">
-        <v>2200</v>
+        <v>162</v>
+      </c>
+      <c r="F17" s="6">
+        <v>3790</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>122</v>
+        <v>86</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1639,10 +1708,10 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1650,26 +1719,26 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="F18" s="7">
-        <v>2200</v>
+        <v>162</v>
+      </c>
+      <c r="F18" s="6">
+        <v>3790</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="H18" s="5"/>
-      <c r="I18" s="5" t="s">
-        <v>123</v>
+      <c r="I18" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
@@ -1677,10 +1746,10 @@
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1688,37 +1757,37 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="F19" s="7">
-        <v>2200</v>
+        <v>162</v>
+      </c>
+      <c r="F19" s="6">
+        <v>3790</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="5" t="s">
-        <v>124</v>
+      <c r="J19" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1726,37 +1795,37 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F20" s="7">
-        <v>2000</v>
+        <v>162</v>
+      </c>
+      <c r="F20" s="6">
+        <v>3790</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>125</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1764,37 +1833,37 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F21" s="7">
-        <v>2000</v>
+        <v>162</v>
+      </c>
+      <c r="F21" s="6">
+        <v>3790</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="I21" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1802,65 +1871,62 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" s="7">
-        <v>4000</v>
+        <v>83</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F22" s="6">
+        <v>3790</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>127</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="M22" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="N22" s="5"/>
       <c r="O22" s="5">
         <v>1</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>151</v>
+      <c r="B23" s="5" t="str">
+        <f t="shared" ref="B23:B24" si="1">+CONCATENATE(C23," ",D23)</f>
+        <v>Ojo de Tigre CRYSTAL SCENTS</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>104</v>
+        <v>199</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F23" s="7">
-        <v>4000</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="6">
+        <v>3790</v>
+      </c>
+      <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="5" t="s">
-        <v>128</v>
-      </c>
+      <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -1870,36 +1936,33 @@
         <v>1</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>152</v>
+      <c r="B24" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Venturina CRYSTAL SCENTS</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F24" s="7">
-        <v>4000</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F24" s="6">
+        <v>3790</v>
+      </c>
+      <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="5" t="s">
-        <v>129</v>
-      </c>
+      <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
@@ -1908,77 +1971,938 @@
         <v>1</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F25" s="6">
+        <v>4290</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5">
+        <v>2</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" s="6">
+        <v>4290</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5">
+        <v>2</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <f t="shared" ref="B27:B28" si="2">+CONCATENATE(C27," ",D27)</f>
+        <v>Watermelon SAGRADA MADRE</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" s="6">
+        <v>4290</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5">
+        <v>2</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>Purple Hindu Kush SAGRADA MADRE</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="6">
+        <v>4290</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5">
+        <v>2</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="7">
+        <v>3690</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5">
+        <v>2</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="str">
+        <f t="shared" ref="B30" si="3">+CONCATENATE(C30," ",D30)</f>
+        <v>Ritual Abundancia SAGRADA MADRE</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F30" s="7">
+        <v>3690</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5">
+        <v>2</v>
+      </c>
+      <c r="P30" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B31" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F31" s="7">
+        <v>3990</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5">
+        <v>0</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F32" s="7">
+        <v>3990</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5">
+        <v>1</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F33" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5">
+        <v>2</v>
+      </c>
+      <c r="P33" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F34" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5">
+        <v>2</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <f t="shared" ref="B35:B37" si="4">+CONCATENATE(C35," ",D35)</f>
+        <v>Naranja Pimienta  AROMANZA</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F35" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5">
+        <v>3</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>Variedad Aromatica AROMANZA</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F36" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5">
+        <v>2</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>Lavanda AROMANZA</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" s="7">
+        <v>2000</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5">
+        <v>2</v>
+      </c>
+      <c r="P37" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F38" s="7">
+        <v>4000</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5">
+        <v>0</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" s="7">
+        <v>4000</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5">
+        <v>0</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F40" s="7">
+        <v>4000</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5">
+        <v>0</v>
+      </c>
+      <c r="P40" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="7">
+        <v>6490</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O41" s="5">
+        <v>0</v>
+      </c>
+      <c r="P41" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F42" s="7">
+        <v>6490</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" s="7">
-        <v>4200</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="O25" s="5">
-        <v>1</v>
-      </c>
-      <c r="P25" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>31</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="I42" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="O42" s="5">
+        <v>0</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="str">
+        <f t="shared" ref="B43:B52" si="5">+CONCATENATE(C43," ",D43)</f>
+        <v>Black Ice XL AROMA FUSION</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F26" s="7">
-        <v>4200</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="O26" s="5">
-        <v>1</v>
-      </c>
-      <c r="P26" s="5" t="s">
-        <v>71</v>
+      <c r="E43" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F43" s="7">
+        <v>6490</v>
+      </c>
+      <c r="O43" s="5">
+        <v>2</v>
+      </c>
+      <c r="P43" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Strawberry XL AROMA FUSION</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F44" s="7">
+        <v>6490</v>
+      </c>
+      <c r="O44" s="5">
+        <v>2</v>
+      </c>
+      <c r="P44" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Cool water AROMA FUSION</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F45" s="7">
+        <v>2000</v>
+      </c>
+      <c r="O45" s="5">
+        <v>2</v>
+      </c>
+      <c r="P45" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Manzana Canela AROMA FUSION</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F46" s="7">
+        <v>2000</v>
+      </c>
+      <c r="O46" s="5">
+        <v>2</v>
+      </c>
+      <c r="P46" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Lavanda  AROMA FUSION</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F47" s="7">
+        <v>2000</v>
+      </c>
+      <c r="O47" s="5">
+        <v>2</v>
+      </c>
+      <c r="P47" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Strawberry  AROMA FUSION</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F48" s="7">
+        <v>2000</v>
+      </c>
+      <c r="O48" s="5">
+        <v>2</v>
+      </c>
+      <c r="P48" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Palo Santo AROMA FUSION</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F49" s="7">
+        <v>2000</v>
+      </c>
+      <c r="O49" s="5">
+        <v>2</v>
+      </c>
+      <c r="P49" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Rosa Vainilla AROMA FUSION</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F50" s="7">
+        <v>2000</v>
+      </c>
+      <c r="O50" s="5">
+        <v>2</v>
+      </c>
+      <c r="P50" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Black Ice  AROMA FUSION</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F51" s="7">
+        <v>2000</v>
+      </c>
+      <c r="O51" s="5">
+        <v>2</v>
+      </c>
+      <c r="P51" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>Sahumerios Surtidos VARIAS</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F52" s="7">
+        <v>1000</v>
+      </c>
+      <c r="O52" s="5">
+        <v>43</v>
+      </c>
+      <c r="P52" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P52"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Agrega fotos de productos
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -1057,7 +1057,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="C34:E43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1589,7 +1591,7 @@
         <v>206</v>
       </c>
       <c r="F14" s="6">
-        <v>4190</v>
+        <v>1890</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1624,7 +1626,7 @@
         <v>206</v>
       </c>
       <c r="F15" s="6">
-        <v>4190</v>
+        <v>1890</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1659,7 +1661,7 @@
         <v>206</v>
       </c>
       <c r="F16" s="6">
-        <v>4190</v>
+        <v>1890</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>

</xml_diff>